<commit_message>
Fixes to creator status page, Creators now recognized in scans, Excels from top rated will display recognized creators.
</commit_message>
<xml_diff>
--- a/UGCOfWorkshopMonth.xlsx
+++ b/UGCOfWorkshopMonth.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="93">
   <si>
     <t>Level</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Language</t>
   </si>
   <si>
-    <t>TUS (2024-05-24)</t>
+    <t>TUS (2024-05-27)</t>
   </si>
   <si>
     <t>Rating</t>
@@ -49,6 +49,24 @@
     <t>Model</t>
   </si>
   <si>
+    <t>Increase The Volume</t>
+  </si>
+  <si>
+    <t>脸红</t>
+  </si>
+  <si>
+    <t>24/05/2024</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>zh-cn</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>墨墨29-春游</t>
   </si>
   <si>
@@ -58,10 +76,7 @@
     <t>18/05/2024</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>zh-cn</t>
+    <t>ko</t>
   </si>
   <si>
     <t>mechanical maze</t>
@@ -73,7 +88,22 @@
     <t>16/05/2024</t>
   </si>
   <si>
-    <t>CN</t>
+    <t>溺梦（连跳）</t>
+  </si>
+  <si>
+    <t>哏</t>
+  </si>
+  <si>
+    <t>19/05/2024</t>
+  </si>
+  <si>
+    <t>养只咩咩</t>
+  </si>
+  <si>
+    <t>35"</t>
+  </si>
+  <si>
+    <t>26/05/2024</t>
   </si>
   <si>
     <t>Mountain</t>
@@ -91,33 +121,147 @@
     <t>时遗 (连跳)</t>
   </si>
   <si>
-    <t>哏</t>
-  </si>
-  <si>
-    <t>溺梦（连跳）</t>
-  </si>
-  <si>
-    <t>19/05/2024</t>
-  </si>
-  <si>
-    <t>yanjing</t>
-  </si>
-  <si>
-    <t>爆爆</t>
-  </si>
-  <si>
-    <t>17/05/2024</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Diaz</t>
+    <t>CANDY WORLD</t>
+  </si>
+  <si>
+    <t>激辣浪味仙☆</t>
+  </si>
+  <si>
+    <t>09/05/2024</t>
+  </si>
+  <si>
+    <t>悬溺</t>
+  </si>
+  <si>
+    <t>ℯℓ.凉cc</t>
+  </si>
+  <si>
+    <t>11/05/2024</t>
+  </si>
+  <si>
+    <t>菜就多练4</t>
+  </si>
+  <si>
+    <t>10/05/2024</t>
+  </si>
+  <si>
+    <t>Granny 3 V2 MAJOR UPDATE</t>
+  </si>
+  <si>
+    <t>RAFA120</t>
+  </si>
+  <si>
+    <t>05/05/2024</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>敢直视我吗 嘿嘿</t>
+  </si>
+  <si>
+    <t>甘九</t>
+  </si>
+  <si>
+    <t>03/05/2024</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>j0hNtWiN</t>
   </si>
   <si>
     <t>pl</t>
   </si>
   <si>
+    <t>Бабиджон</t>
+  </si>
+  <si>
+    <t>PonosUzbeka228</t>
+  </si>
+  <si>
+    <t>ru</t>
+  </si>
+  <si>
+    <t>DOVE</t>
+  </si>
+  <si>
+    <t>香脆小条</t>
+  </si>
+  <si>
+    <t>25/05/2024</t>
+  </si>
+  <si>
+    <t>AMONG ussss 2</t>
+  </si>
+  <si>
+    <t>3keysteve</t>
+  </si>
+  <si>
+    <t>22/05/2024</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Faust</t>
+  </si>
+  <si>
+    <t>还是处</t>
+  </si>
+  <si>
+    <t>27/05/2024</t>
+  </si>
+  <si>
+    <t>Maga</t>
+  </si>
+  <si>
+    <t>Mythi</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>sw</t>
+  </si>
+  <si>
+    <t>sigma dany</t>
+  </si>
+  <si>
+    <t>dany</t>
+  </si>
+  <si>
+    <t>so</t>
+  </si>
+  <si>
+    <t>AlexLebeau</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>Meneer Özbel</t>
+  </si>
+  <si>
+    <t>Alezei</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>pumknight</t>
+  </si>
+  <si>
+    <t>PappieMcaffe</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
     <t>Chucken</t>
   </si>
   <si>
@@ -130,20 +274,32 @@
     <t>PL</t>
   </si>
   <si>
-    <t>de</t>
-  </si>
-  <si>
     <t>RockyDoggy</t>
   </si>
   <si>
     <t>Maxplaier</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>s1mple</t>
+  </si>
+  <si>
+    <t>Agent 69</t>
+  </si>
+  <si>
+    <t>RedBear</t>
+  </si>
+  <si>
+    <t>tr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,13 +307,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -172,8 +355,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +653,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -515,7 +700,7 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
@@ -528,13 +713,13 @@
         <v>15</v>
       </c>
       <c r="G3">
-        <v>393</v>
+        <v>412</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -542,28 +727,28 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
         <v>17</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G4">
-        <v>1020</v>
+        <v>813</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -571,28 +756,28 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
         <v>21</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G5">
-        <v>312</v>
+        <v>1775</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -602,26 +787,26 @@
       <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
       </c>
       <c r="G6">
-        <v>87</v>
+        <v>175</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -629,207 +814,697 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
       </c>
       <c r="G7">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>10</v>
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8">
+        <v>417</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>1</v>
+      <c r="A9">
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>113</v>
       </c>
       <c r="H9" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G10">
-        <v>221</v>
+        <v>3365</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G11">
-        <v>104</v>
+        <v>226</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
+        <v>41</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="G12">
-        <v>6</v>
+        <v>148</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
+        <v>43</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F13" t="s">
         <v>33</v>
       </c>
       <c r="G13">
-        <v>4</v>
+        <v>1249</v>
       </c>
       <c r="H13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <v>655</v>
+      </c>
+      <c r="H14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
         <v>5</v>
       </c>
-      <c r="B14" t="s">
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17">
+        <v>29</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18">
+        <v>22</v>
+      </c>
+      <c r="H18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19">
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20">
         <v>40</v>
       </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F22" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>72</v>
+      </c>
+      <c r="G23">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" t="s">
+        <v>78</v>
+      </c>
+      <c r="G25">
+        <v>6</v>
+      </c>
+      <c r="H25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" t="s">
         <v>33</v>
       </c>
-      <c r="G14">
-        <v>5</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="G26">
         <v>14</v>
       </c>
-      <c r="I14" t="s">
+      <c r="H26" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27">
+        <v>11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27">
+        <v>17</v>
+      </c>
+      <c r="H27" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+      <c r="F28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28">
+        <v>9</v>
+      </c>
+      <c r="H28" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" t="s">
+        <v>52</v>
+      </c>
+      <c r="G29">
         <v>14</v>
+      </c>
+      <c r="H29" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30">
+        <v>15</v>
+      </c>
+      <c r="H30" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31">
+        <v>27</v>
+      </c>
+      <c r="H31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>